<commit_message>
Fix train not stable issue Add more adv2
</commit_message>
<xml_diff>
--- a/playground/summary.xlsx
+++ b/playground/summary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8BE78E-9A9B-459F-A029-37F7C79DE61C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF031BE-E0A2-4802-9A55-005A69A9ADA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="ParamsOpt" sheetId="6" r:id="rId6"/>
     <sheet name="Submissions" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Submissions!$A$5:$L$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="154">
   <si>
     <t>BaseLine</t>
   </si>
@@ -453,9 +456,6 @@
     <t>T6</t>
   </si>
   <si>
-    <t>T7</t>
-  </si>
-  <si>
     <t>keras_xception_19</t>
   </si>
   <si>
@@ -478,6 +478,24 @@
   </si>
   <si>
     <t>n2.3.7</t>
+  </si>
+  <si>
+    <t>Adv train</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loss and acc jump rapidly when shuffling,  </t>
+  </si>
+  <si>
+    <t>need small learning rate</t>
+  </si>
+  <si>
+    <t>Transfer train</t>
+  </si>
+  <si>
+    <t>adv trained</t>
+  </si>
+  <si>
+    <t>T11</t>
   </si>
 </sst>
 </file>
@@ -1980,10 +1998,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8256FD00-8941-42ED-8238-21974BCCED96}">
-  <dimension ref="B2:D15"/>
+  <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2055,6 +2073,22 @@
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2136,10 +2170,10 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" t="s">
         <v>145</v>
-      </c>
-      <c r="C10" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2218,7 +2252,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,6 +2265,7 @@
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" customWidth="1"/>
     <col min="12" max="12" width="38.140625" customWidth="1"/>
   </cols>
@@ -2255,7 +2290,7 @@
         <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2272,7 +2307,12 @@
         <v>124</v>
       </c>
       <c r="J2" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2411,7 +2451,7 @@
         <v>138</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="H10">
         <v>16</v>
@@ -2431,10 +2471,10 @@
         <v>138</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" t="s">
         <v>142</v>
-      </c>
-      <c r="E11" t="s">
-        <v>143</v>
       </c>
       <c r="H11">
         <v>16</v>
@@ -2443,7 +2483,7 @@
         <v>2.65</v>
       </c>
       <c r="L11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2451,10 +2491,10 @@
         <v>3.8</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>125</v>
@@ -2471,8 +2511,12 @@
       <c r="H12">
         <v>16</v>
       </c>
+      <c r="K12">
+        <v>49.81</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A5:L5" xr:uid="{4FDFD235-02C0-4226-93DA-D0F7EBC75763}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>